<commit_message>
improved crowding + init by heuristic
crowding is improved but slow
possibility to initialize population with heuristic
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\School\FIRW MAI\Genetic Algorithms\Project-TSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8502870F-D540-409E-8D7B-88B0DA40CF91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70F2701-DB68-47BE-9B6A-9B76056D9D75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-3300" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t xml:space="preserve">Value </t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>greedy</t>
+  </si>
+  <si>
+    <t>popsize=250, offspring=150, k=5, alpha=0.05, prc=0.99, crowding (chance:0.5, hammingdistance)</t>
   </si>
 </sst>
 </file>
@@ -538,7 +541,7 @@
   <dimension ref="B2:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,9 +594,17 @@
       <c r="C5" s="5">
         <v>27200</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="6">
+        <f>AVERAGE(28377, 28907, 29424)</f>
+        <v>28902.666666666668</v>
+      </c>
+      <c r="F5" s="7">
+        <f>AVERAGE(51.79, 62.86, 48.13,38.67)</f>
+        <v>50.362499999999997</v>
+      </c>
       <c r="J5">
         <v>1</v>
       </c>
@@ -615,6 +626,12 @@
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="22"/>

</xml_diff>